<commit_message>
added market aware advance rate calculation but works weird
</commit_message>
<xml_diff>
--- a/graphs_caseA.xlsx
+++ b/graphs_caseA.xlsx
@@ -29,186 +29,180 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="166">
-  <si>
-    <t>[3.558-3.583]</t>
-  </si>
-  <si>
-    <t>[3.583-3.608]</t>
-  </si>
-  <si>
-    <t>[3.608-3.633]</t>
-  </si>
-  <si>
-    <t>[3.633-3.657]</t>
-  </si>
-  <si>
-    <t>[3.657-3.682]</t>
-  </si>
-  <si>
-    <t>[3.682-3.707]</t>
-  </si>
-  <si>
-    <t>[3.707-3.732]</t>
-  </si>
-  <si>
-    <t>[3.732-3.757]</t>
-  </si>
-  <si>
-    <t>[3.757-3.782]</t>
-  </si>
-  <si>
-    <t>[3.782-3.806]</t>
-  </si>
-  <si>
-    <t>[3.806-3.831]</t>
-  </si>
-  <si>
-    <t>[3.831-3.856]</t>
-  </si>
-  <si>
-    <t>[3.856-3.881]</t>
-  </si>
-  <si>
-    <t>[3.881-3.906]</t>
-  </si>
-  <si>
-    <t>[3.57-3.585]</t>
-  </si>
-  <si>
-    <t>[3.585-3.6]</t>
-  </si>
-  <si>
-    <t>[3.6-3.615]</t>
-  </si>
-  <si>
-    <t>[3.615-3.63]</t>
-  </si>
-  <si>
-    <t>[3.63-3.644]</t>
-  </si>
-  <si>
-    <t>[3.644-3.659]</t>
-  </si>
-  <si>
-    <t>[3.659-3.674]</t>
-  </si>
-  <si>
-    <t>[3.674-3.689]</t>
-  </si>
-  <si>
-    <t>[3.689-3.704]</t>
-  </si>
-  <si>
-    <t>[3.704-3.718]</t>
-  </si>
-  <si>
-    <t>[3.718-3.733]</t>
-  </si>
-  <si>
-    <t>[3.733-3.748]</t>
-  </si>
-  <si>
-    <t>[3.748-3.763]</t>
-  </si>
-  <si>
-    <t>[3.763-3.778]</t>
-  </si>
-  <si>
-    <t>[3.628-3.648]</t>
-  </si>
-  <si>
-    <t>[3.648-3.667]</t>
-  </si>
-  <si>
-    <t>[3.667-3.687]</t>
-  </si>
-  <si>
-    <t>[3.687-3.707]</t>
-  </si>
-  <si>
-    <t>[3.707-3.727]</t>
-  </si>
-  <si>
-    <t>[3.727-3.747]</t>
-  </si>
-  <si>
-    <t>[3.747-3.767]</t>
-  </si>
-  <si>
-    <t>[3.767-3.787]</t>
-  </si>
-  <si>
-    <t>[3.787-3.806]</t>
-  </si>
-  <si>
-    <t>[3.806-3.826]</t>
-  </si>
-  <si>
-    <t>[3.826-3.846]</t>
-  </si>
-  <si>
-    <t>[3.846-3.866]</t>
-  </si>
-  <si>
-    <t>[3.866-3.886]</t>
-  </si>
-  <si>
-    <t>[3.886-3.906]</t>
-  </si>
-  <si>
-    <t>[3.558-3.572]</t>
-  </si>
-  <si>
-    <t>[3.572-3.585]</t>
-  </si>
-  <si>
-    <t>[3.585-3.599]</t>
-  </si>
-  <si>
-    <t>[3.599-3.613]</t>
-  </si>
-  <si>
-    <t>[3.613-3.626]</t>
-  </si>
-  <si>
-    <t>[3.626-3.64]</t>
-  </si>
-  <si>
-    <t>[3.64-3.654]</t>
-  </si>
-  <si>
-    <t>[3.654-3.667]</t>
-  </si>
-  <si>
-    <t>[3.667-3.681]</t>
-  </si>
-  <si>
-    <t>[3.681-3.694]</t>
-  </si>
-  <si>
-    <t>[3.694-3.708]</t>
-  </si>
-  <si>
-    <t>[3.708-3.722]</t>
-  </si>
-  <si>
-    <t>[3.722-3.735]</t>
-  </si>
-  <si>
-    <t>[3.735-3.749]</t>
-  </si>
-  <si>
-    <t>[10.78-10.92]</t>
-  </si>
-  <si>
-    <t>[10.92-11.07]</t>
-  </si>
-  <si>
-    <t>[11.07-11.22]</t>
-  </si>
-  <si>
-    <t>[11.22-11.37]</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+  <si>
+    <t>[3.471-3.504]</t>
+  </si>
+  <si>
+    <t>[3.504-3.536]</t>
+  </si>
+  <si>
+    <t>[3.536-3.568]</t>
+  </si>
+  <si>
+    <t>[3.568-3.6]</t>
+  </si>
+  <si>
+    <t>[3.6-3.632]</t>
+  </si>
+  <si>
+    <t>[3.632-3.664]</t>
+  </si>
+  <si>
+    <t>[3.664-3.697]</t>
+  </si>
+  <si>
+    <t>[3.697-3.729]</t>
+  </si>
+  <si>
+    <t>[3.729-3.761]</t>
+  </si>
+  <si>
+    <t>[3.761-3.793]</t>
+  </si>
+  <si>
+    <t>[3.793-3.825]</t>
+  </si>
+  <si>
+    <t>[3.825-3.858]</t>
+  </si>
+  <si>
+    <t>[3.858-3.89]</t>
+  </si>
+  <si>
+    <t>[3.89-3.922]</t>
+  </si>
+  <si>
+    <t>[3.471-3.493]</t>
+  </si>
+  <si>
+    <t>[3.493-3.515]</t>
+  </si>
+  <si>
+    <t>[3.515-3.537]</t>
+  </si>
+  <si>
+    <t>[3.537-3.559]</t>
+  </si>
+  <si>
+    <t>[3.559-3.582]</t>
+  </si>
+  <si>
+    <t>[3.582-3.604]</t>
+  </si>
+  <si>
+    <t>[3.604-3.626]</t>
+  </si>
+  <si>
+    <t>[3.626-3.648]</t>
+  </si>
+  <si>
+    <t>[3.648-3.67]</t>
+  </si>
+  <si>
+    <t>[3.67-3.692]</t>
+  </si>
+  <si>
+    <t>[3.692-3.714]</t>
+  </si>
+  <si>
+    <t>[3.714-3.736]</t>
+  </si>
+  <si>
+    <t>[3.736-3.758]</t>
+  </si>
+  <si>
+    <t>[3.758-3.78]</t>
+  </si>
+  <si>
+    <t>[3.555-3.581]</t>
+  </si>
+  <si>
+    <t>[3.581-3.607]</t>
+  </si>
+  <si>
+    <t>[3.607-3.633]</t>
+  </si>
+  <si>
+    <t>[3.633-3.66]</t>
+  </si>
+  <si>
+    <t>[3.66-3.686]</t>
+  </si>
+  <si>
+    <t>[3.686-3.712]</t>
+  </si>
+  <si>
+    <t>[3.712-3.738]</t>
+  </si>
+  <si>
+    <t>[3.738-3.764]</t>
+  </si>
+  <si>
+    <t>[3.764-3.791]</t>
+  </si>
+  <si>
+    <t>[3.791-3.817]</t>
+  </si>
+  <si>
+    <t>[3.817-3.843]</t>
+  </si>
+  <si>
+    <t>[3.843-3.869]</t>
+  </si>
+  <si>
+    <t>[3.869-3.896]</t>
+  </si>
+  <si>
+    <t>[3.896-3.922]</t>
+  </si>
+  <si>
+    <t>[3.481-3.502]</t>
+  </si>
+  <si>
+    <t>[3.502-3.523]</t>
+  </si>
+  <si>
+    <t>[3.523-3.544]</t>
+  </si>
+  <si>
+    <t>[3.544-3.564]</t>
+  </si>
+  <si>
+    <t>[3.564-3.585]</t>
+  </si>
+  <si>
+    <t>[3.585-3.606]</t>
+  </si>
+  <si>
+    <t>[3.606-3.627]</t>
+  </si>
+  <si>
+    <t>[3.627-3.648]</t>
+  </si>
+  <si>
+    <t>[3.648-3.669]</t>
+  </si>
+  <si>
+    <t>[3.669-3.69]</t>
+  </si>
+  <si>
+    <t>[3.69-3.71]</t>
+  </si>
+  <si>
+    <t>[3.71-3.731]</t>
+  </si>
+  <si>
+    <t>[3.731-3.752]</t>
+  </si>
+  <si>
+    <t>[3.752-3.773]</t>
+  </si>
+  <si>
+    <t>[11.08-11.23]</t>
+  </si>
+  <si>
+    <t>[11.23-11.37]</t>
   </si>
   <si>
     <t>[11.37-11.52]</t>
@@ -241,292 +235,304 @@
     <t>[12.71-12.86]</t>
   </si>
   <si>
-    <t>[11.54-11.63]</t>
-  </si>
-  <si>
-    <t>[11.63-11.72]</t>
-  </si>
-  <si>
-    <t>[11.72-11.81]</t>
-  </si>
-  <si>
-    <t>[11.81-11.9]</t>
-  </si>
-  <si>
-    <t>[11.9-11.98]</t>
-  </si>
-  <si>
-    <t>[11.98-12.07]</t>
-  </si>
-  <si>
-    <t>[12.07-12.16]</t>
-  </si>
-  <si>
-    <t>[12.16-12.25]</t>
-  </si>
-  <si>
-    <t>[12.25-12.34]</t>
-  </si>
-  <si>
-    <t>[12.34-12.43]</t>
-  </si>
-  <si>
-    <t>[12.43-12.52]</t>
-  </si>
-  <si>
-    <t>[12.52-12.6]</t>
-  </si>
-  <si>
-    <t>[12.6-12.69]</t>
-  </si>
-  <si>
-    <t>[12.69-12.78]</t>
-  </si>
-  <si>
-    <t>[10.78-10.9]</t>
-  </si>
-  <si>
-    <t>[10.9-11.01]</t>
-  </si>
-  <si>
-    <t>[11.01-11.13]</t>
-  </si>
-  <si>
-    <t>[11.13-11.25]</t>
-  </si>
-  <si>
-    <t>[11.25-11.37]</t>
-  </si>
-  <si>
-    <t>[11.37-11.49]</t>
-  </si>
-  <si>
-    <t>[11.49-11.61]</t>
-  </si>
-  <si>
-    <t>[11.61-11.73]</t>
-  </si>
-  <si>
-    <t>[11.73-11.85]</t>
-  </si>
-  <si>
-    <t>[11.85-11.96]</t>
-  </si>
-  <si>
-    <t>[11.96-12.08]</t>
-  </si>
-  <si>
-    <t>[12.08-12.2]</t>
-  </si>
-  <si>
-    <t>[12.2-12.32]</t>
-  </si>
-  <si>
-    <t>[12.32-12.44]</t>
-  </si>
-  <si>
-    <t>[11.71-11.79]</t>
-  </si>
-  <si>
-    <t>[11.79-11.88]</t>
-  </si>
-  <si>
-    <t>[11.88-11.96]</t>
-  </si>
-  <si>
-    <t>[11.96-12.04]</t>
-  </si>
-  <si>
-    <t>[12.04-12.12]</t>
-  </si>
-  <si>
-    <t>[12.12-12.2]</t>
-  </si>
-  <si>
-    <t>[12.2-12.28]</t>
-  </si>
-  <si>
-    <t>[12.28-12.37]</t>
-  </si>
-  <si>
-    <t>[12.37-12.45]</t>
-  </si>
-  <si>
-    <t>[12.45-12.53]</t>
-  </si>
-  <si>
-    <t>[12.53-12.61]</t>
-  </si>
-  <si>
-    <t>[12.61-12.69]</t>
-  </si>
-  <si>
-    <t>[12.78-12.86]</t>
-  </si>
-  <si>
-    <t>[83.31-83.45]</t>
-  </si>
-  <si>
-    <t>[83.45-83.6]</t>
-  </si>
-  <si>
-    <t>[83.6-83.74]</t>
-  </si>
-  <si>
-    <t>[83.74-83.89]</t>
-  </si>
-  <si>
-    <t>[83.89-84.03]</t>
-  </si>
-  <si>
-    <t>[84.03-84.18]</t>
-  </si>
-  <si>
-    <t>[84.18-84.32]</t>
-  </si>
-  <si>
-    <t>[84.32-84.47]</t>
-  </si>
-  <si>
-    <t>[84.47-84.61]</t>
-  </si>
-  <si>
-    <t>[84.61-84.76]</t>
-  </si>
-  <si>
-    <t>[84.76-84.9]</t>
-  </si>
-  <si>
-    <t>[84.9-85.04]</t>
-  </si>
-  <si>
-    <t>[85.04-85.19]</t>
-  </si>
-  <si>
-    <t>[85.19-85.33]</t>
-  </si>
-  <si>
-    <t>[83.48-83.6]</t>
-  </si>
-  <si>
-    <t>[83.6-83.73]</t>
-  </si>
-  <si>
-    <t>[83.73-83.85]</t>
-  </si>
-  <si>
-    <t>[83.85-83.98]</t>
-  </si>
-  <si>
-    <t>[83.98-84.1]</t>
-  </si>
-  <si>
-    <t>[84.1-84.23]</t>
-  </si>
-  <si>
-    <t>[84.23-84.35]</t>
-  </si>
-  <si>
-    <t>[84.35-84.48]</t>
-  </si>
-  <si>
-    <t>[84.48-84.6]</t>
-  </si>
-  <si>
-    <t>[84.6-84.73]</t>
-  </si>
-  <si>
-    <t>[84.73-84.85]</t>
-  </si>
-  <si>
-    <t>[84.85-84.98]</t>
-  </si>
-  <si>
-    <t>[84.98-85.1]</t>
-  </si>
-  <si>
-    <t>[85.1-85.23]</t>
-  </si>
-  <si>
-    <t>[83.31-83.43]</t>
-  </si>
-  <si>
-    <t>[83.43-83.55]</t>
-  </si>
-  <si>
-    <t>[83.55-83.67]</t>
-  </si>
-  <si>
-    <t>[83.67-83.79]</t>
-  </si>
-  <si>
-    <t>[83.79-83.91]</t>
-  </si>
-  <si>
-    <t>[83.91-84.03]</t>
-  </si>
-  <si>
-    <t>[84.03-84.15]</t>
-  </si>
-  <si>
-    <t>[84.15-84.27]</t>
-  </si>
-  <si>
-    <t>[84.27-84.39]</t>
-  </si>
-  <si>
-    <t>[84.39-84.51]</t>
-  </si>
-  <si>
-    <t>[84.51-84.63]</t>
-  </si>
-  <si>
-    <t>[84.63-84.75]</t>
-  </si>
-  <si>
-    <t>[84.75-84.87]</t>
-  </si>
-  <si>
-    <t>[84.87-84.99]</t>
-  </si>
-  <si>
-    <t>[83.64-83.76]</t>
-  </si>
-  <si>
-    <t>[83.76-83.88]</t>
-  </si>
-  <si>
-    <t>[83.88-84.0]</t>
-  </si>
-  <si>
-    <t>[84.0-84.12]</t>
-  </si>
-  <si>
-    <t>[84.12-84.24]</t>
-  </si>
-  <si>
-    <t>[84.24-84.36]</t>
-  </si>
-  <si>
-    <t>[84.36-84.48]</t>
-  </si>
-  <si>
-    <t>[84.48-84.61]</t>
-  </si>
-  <si>
-    <t>[84.61-84.73]</t>
-  </si>
-  <si>
-    <t>[84.85-84.97]</t>
-  </si>
-  <si>
-    <t>[84.97-85.09]</t>
-  </si>
-  <si>
-    <t>[85.09-85.21]</t>
-  </si>
-  <si>
-    <t>[85.21-85.33]</t>
+    <t>[12.86-13.0]</t>
+  </si>
+  <si>
+    <t>[13.0-13.15]</t>
+  </si>
+  <si>
+    <t>[11.71-11.81]</t>
+  </si>
+  <si>
+    <t>[11.81-11.91]</t>
+  </si>
+  <si>
+    <t>[11.91-12.02]</t>
+  </si>
+  <si>
+    <t>[12.02-12.12]</t>
+  </si>
+  <si>
+    <t>[12.12-12.22]</t>
+  </si>
+  <si>
+    <t>[12.22-12.33]</t>
+  </si>
+  <si>
+    <t>[12.33-12.43]</t>
+  </si>
+  <si>
+    <t>[12.43-12.53]</t>
+  </si>
+  <si>
+    <t>[12.53-12.64]</t>
+  </si>
+  <si>
+    <t>[12.64-12.74]</t>
+  </si>
+  <si>
+    <t>[12.74-12.84]</t>
+  </si>
+  <si>
+    <t>[12.84-12.95]</t>
+  </si>
+  <si>
+    <t>[12.95-13.05]</t>
+  </si>
+  <si>
+    <t>[13.05-13.15]</t>
+  </si>
+  <si>
+    <t>[11.08-11.2]</t>
+  </si>
+  <si>
+    <t>[11.2-11.32]</t>
+  </si>
+  <si>
+    <t>[11.32-11.44]</t>
+  </si>
+  <si>
+    <t>[11.44-11.56]</t>
+  </si>
+  <si>
+    <t>[11.56-11.68]</t>
+  </si>
+  <si>
+    <t>[11.68-11.8]</t>
+  </si>
+  <si>
+    <t>[11.8-11.92]</t>
+  </si>
+  <si>
+    <t>[11.92-12.04]</t>
+  </si>
+  <si>
+    <t>[12.04-12.16]</t>
+  </si>
+  <si>
+    <t>[12.16-12.28]</t>
+  </si>
+  <si>
+    <t>[12.28-12.4]</t>
+  </si>
+  <si>
+    <t>[12.4-12.52]</t>
+  </si>
+  <si>
+    <t>[12.52-12.65]</t>
+  </si>
+  <si>
+    <t>[12.65-12.77]</t>
+  </si>
+  <si>
+    <t>[11.73-11.83]</t>
+  </si>
+  <si>
+    <t>[11.83-11.93]</t>
+  </si>
+  <si>
+    <t>[11.93-12.03]</t>
+  </si>
+  <si>
+    <t>[12.03-12.13]</t>
+  </si>
+  <si>
+    <t>[12.13-12.23]</t>
+  </si>
+  <si>
+    <t>[12.23-12.32]</t>
+  </si>
+  <si>
+    <t>[12.32-12.42]</t>
+  </si>
+  <si>
+    <t>[12.42-12.52]</t>
+  </si>
+  <si>
+    <t>[12.52-12.62]</t>
+  </si>
+  <si>
+    <t>[12.62-12.72]</t>
+  </si>
+  <si>
+    <t>[12.72-12.82]</t>
+  </si>
+  <si>
+    <t>[12.82-12.92]</t>
+  </si>
+  <si>
+    <t>[12.92-13.02]</t>
+  </si>
+  <si>
+    <t>[13.02-13.12]</t>
+  </si>
+  <si>
+    <t>[78.83-79.04]</t>
+  </si>
+  <si>
+    <t>[79.04-79.24]</t>
+  </si>
+  <si>
+    <t>[79.24-79.44]</t>
+  </si>
+  <si>
+    <t>[79.44-79.64]</t>
+  </si>
+  <si>
+    <t>[79.64-79.84]</t>
+  </si>
+  <si>
+    <t>[79.84-80.04]</t>
+  </si>
+  <si>
+    <t>[80.04-80.24]</t>
+  </si>
+  <si>
+    <t>[80.24-80.44]</t>
+  </si>
+  <si>
+    <t>[80.44-80.64]</t>
+  </si>
+  <si>
+    <t>[80.64-80.84]</t>
+  </si>
+  <si>
+    <t>[80.84-81.04]</t>
+  </si>
+  <si>
+    <t>[81.04-81.24]</t>
+  </si>
+  <si>
+    <t>[81.24-81.44]</t>
+  </si>
+  <si>
+    <t>[81.44-81.64]</t>
+  </si>
+  <si>
+    <t>[79.34-79.5]</t>
+  </si>
+  <si>
+    <t>[79.5-79.67]</t>
+  </si>
+  <si>
+    <t>[79.67-79.83]</t>
+  </si>
+  <si>
+    <t>[79.83-80.0]</t>
+  </si>
+  <si>
+    <t>[80.0-80.16]</t>
+  </si>
+  <si>
+    <t>[80.16-80.33]</t>
+  </si>
+  <si>
+    <t>[80.33-80.49]</t>
+  </si>
+  <si>
+    <t>[80.49-80.65]</t>
+  </si>
+  <si>
+    <t>[80.65-80.82]</t>
+  </si>
+  <si>
+    <t>[80.82-80.98]</t>
+  </si>
+  <si>
+    <t>[80.98-81.15]</t>
+  </si>
+  <si>
+    <t>[81.15-81.31]</t>
+  </si>
+  <si>
+    <t>[81.31-81.48]</t>
+  </si>
+  <si>
+    <t>[81.48-81.64]</t>
+  </si>
+  <si>
+    <t>[78.83-79.03]</t>
+  </si>
+  <si>
+    <t>[79.03-79.23]</t>
+  </si>
+  <si>
+    <t>[79.23-79.42]</t>
+  </si>
+  <si>
+    <t>[79.42-79.62]</t>
+  </si>
+  <si>
+    <t>[79.62-79.81]</t>
+  </si>
+  <si>
+    <t>[79.81-80.01]</t>
+  </si>
+  <si>
+    <t>[80.01-80.2]</t>
+  </si>
+  <si>
+    <t>[80.2-80.4]</t>
+  </si>
+  <si>
+    <t>[80.4-80.59]</t>
+  </si>
+  <si>
+    <t>[80.59-80.79]</t>
+  </si>
+  <si>
+    <t>[80.79-80.99]</t>
+  </si>
+  <si>
+    <t>[80.99-81.18]</t>
+  </si>
+  <si>
+    <t>[81.18-81.38]</t>
+  </si>
+  <si>
+    <t>[81.38-81.57]</t>
+  </si>
+  <si>
+    <t>[79.11-79.28]</t>
+  </si>
+  <si>
+    <t>[79.28-79.46]</t>
+  </si>
+  <si>
+    <t>[79.46-79.64]</t>
+  </si>
+  <si>
+    <t>[79.64-79.82]</t>
+  </si>
+  <si>
+    <t>[79.82-80.0]</t>
+  </si>
+  <si>
+    <t>[80.0-80.17]</t>
+  </si>
+  <si>
+    <t>[80.17-80.35]</t>
+  </si>
+  <si>
+    <t>[80.35-80.53]</t>
+  </si>
+  <si>
+    <t>[80.53-80.71]</t>
+  </si>
+  <si>
+    <t>[80.71-80.89]</t>
+  </si>
+  <si>
+    <t>[80.89-81.06]</t>
+  </si>
+  <si>
+    <t>[81.06-81.24]</t>
+  </si>
+  <si>
+    <t>[81.24-81.42]</t>
+  </si>
+  <si>
+    <t>[81.42-81.6]</t>
   </si>
 </sst>
 </file>
@@ -632,31 +638,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>25</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
                 <c:pt idx="8">
-                  <c:v>35</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -668,31 +674,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>4</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>41</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>53</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>111</c:v>
+                  <c:v>79</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>38</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -819,46 +825,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[11.54-11.63]</c:v>
+                  <c:v>[11.71-11.81]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[11.63-11.72]</c:v>
+                  <c:v>[11.81-11.91]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[11.72-11.81]</c:v>
+                  <c:v>[11.91-12.02]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[11.81-11.9]</c:v>
+                  <c:v>[12.02-12.12]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[11.9-11.98]</c:v>
+                  <c:v>[12.12-12.22]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[11.98-12.07]</c:v>
+                  <c:v>[12.22-12.33]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[12.07-12.16]</c:v>
+                  <c:v>[12.33-12.43]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[12.16-12.25]</c:v>
+                  <c:v>[12.43-12.53]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[12.25-12.34]</c:v>
+                  <c:v>[12.53-12.64]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[12.34-12.43]</c:v>
+                  <c:v>[12.64-12.74]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[12.43-12.52]</c:v>
+                  <c:v>[12.74-12.84]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[12.52-12.6]</c:v>
+                  <c:v>[12.84-12.95]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[12.6-12.69]</c:v>
+                  <c:v>[12.95-13.05]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[12.69-12.78]</c:v>
+                  <c:v>[13.05-13.15]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -873,43 +879,43 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="9">
                   <c:v>16</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1046,46 +1052,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[10.78-10.9]</c:v>
+                  <c:v>[11.08-11.2]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[10.9-11.01]</c:v>
+                  <c:v>[11.2-11.32]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[11.01-11.13]</c:v>
+                  <c:v>[11.32-11.44]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[11.13-11.25]</c:v>
+                  <c:v>[11.44-11.56]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[11.25-11.37]</c:v>
+                  <c:v>[11.56-11.68]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[11.37-11.49]</c:v>
+                  <c:v>[11.68-11.8]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[11.49-11.61]</c:v>
+                  <c:v>[11.8-11.92]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[11.61-11.73]</c:v>
+                  <c:v>[11.92-12.04]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[11.73-11.85]</c:v>
+                  <c:v>[12.04-12.16]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[11.85-11.96]</c:v>
+                  <c:v>[12.16-12.28]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[11.96-12.08]</c:v>
+                  <c:v>[12.28-12.4]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[12.08-12.2]</c:v>
+                  <c:v>[12.4-12.52]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[12.2-12.32]</c:v>
+                  <c:v>[12.52-12.65]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[12.32-12.44]</c:v>
+                  <c:v>[12.65-12.77]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1097,46 +1103,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>11</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>11</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1273,46 +1279,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[11.71-11.79]</c:v>
+                  <c:v>[11.73-11.83]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[11.79-11.88]</c:v>
+                  <c:v>[11.83-11.93]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[11.88-11.96]</c:v>
+                  <c:v>[11.93-12.03]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[11.96-12.04]</c:v>
+                  <c:v>[12.03-12.13]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[12.04-12.12]</c:v>
+                  <c:v>[12.13-12.23]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[12.12-12.2]</c:v>
+                  <c:v>[12.23-12.32]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[12.2-12.28]</c:v>
+                  <c:v>[12.32-12.42]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[12.28-12.37]</c:v>
+                  <c:v>[12.42-12.52]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[12.37-12.45]</c:v>
+                  <c:v>[12.52-12.62]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[12.45-12.53]</c:v>
+                  <c:v>[12.62-12.72]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[12.53-12.61]</c:v>
+                  <c:v>[12.72-12.82]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[12.61-12.69]</c:v>
+                  <c:v>[12.82-12.92]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[12.69-12.78]</c:v>
+                  <c:v>[12.92-13.02]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[12.78-12.86]</c:v>
+                  <c:v>[13.02-13.12]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1324,43 +1330,43 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>13</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>2</c:v>
@@ -1500,46 +1506,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[83.31-83.45]</c:v>
+                  <c:v>[78.83-79.04]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[83.45-83.6]</c:v>
+                  <c:v>[79.04-79.24]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[83.6-83.74]</c:v>
+                  <c:v>[79.24-79.44]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[83.74-83.89]</c:v>
+                  <c:v>[79.44-79.64]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[83.89-84.03]</c:v>
+                  <c:v>[79.64-79.84]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[84.03-84.18]</c:v>
+                  <c:v>[79.84-80.04]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[84.18-84.32]</c:v>
+                  <c:v>[80.04-80.24]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[84.32-84.47]</c:v>
+                  <c:v>[80.24-80.44]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[84.47-84.61]</c:v>
+                  <c:v>[80.44-80.64]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[84.61-84.76]</c:v>
+                  <c:v>[80.64-80.84]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[84.76-84.9]</c:v>
+                  <c:v>[80.84-81.04]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[84.9-85.04]</c:v>
+                  <c:v>[81.04-81.24]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[85.04-85.19]</c:v>
+                  <c:v>[81.24-81.44]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[85.19-85.33]</c:v>
+                  <c:v>[81.44-81.64]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1551,46 +1557,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>13</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20</c:v>
-                </c:pt>
                 <c:pt idx="5">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>32</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>28</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>54</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>30</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1727,46 +1733,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[83.48-83.6]</c:v>
+                  <c:v>[79.34-79.5]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[83.6-83.73]</c:v>
+                  <c:v>[79.5-79.67]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[83.73-83.85]</c:v>
+                  <c:v>[79.67-79.83]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[83.85-83.98]</c:v>
+                  <c:v>[79.83-80.0]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[83.98-84.1]</c:v>
+                  <c:v>[80.0-80.16]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[84.1-84.23]</c:v>
+                  <c:v>[80.16-80.33]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[84.23-84.35]</c:v>
+                  <c:v>[80.33-80.49]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[84.35-84.48]</c:v>
+                  <c:v>[80.49-80.65]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[84.48-84.6]</c:v>
+                  <c:v>[80.65-80.82]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[84.6-84.73]</c:v>
+                  <c:v>[80.82-80.98]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[84.73-84.85]</c:v>
+                  <c:v>[80.98-81.15]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[84.85-84.98]</c:v>
+                  <c:v>[81.15-81.31]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[84.98-85.1]</c:v>
+                  <c:v>[81.31-81.48]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[85.1-85.23]</c:v>
+                  <c:v>[81.48-81.64]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1778,25 +1784,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>13</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>11</c:v>
@@ -1805,13 +1811,13 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>12</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2</c:v>
@@ -1954,46 +1960,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[83.31-83.43]</c:v>
+                  <c:v>[78.83-79.03]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[83.43-83.55]</c:v>
+                  <c:v>[79.03-79.23]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[83.55-83.67]</c:v>
+                  <c:v>[79.23-79.42]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[83.67-83.79]</c:v>
+                  <c:v>[79.42-79.62]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[83.79-83.91]</c:v>
+                  <c:v>[79.62-79.81]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[83.91-84.03]</c:v>
+                  <c:v>[79.81-80.01]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[84.03-84.15]</c:v>
+                  <c:v>[80.01-80.2]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[84.15-84.27]</c:v>
+                  <c:v>[80.2-80.4]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[84.27-84.39]</c:v>
+                  <c:v>[80.4-80.59]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[84.39-84.51]</c:v>
+                  <c:v>[80.59-80.79]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[84.51-84.63]</c:v>
+                  <c:v>[80.79-80.99]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[84.63-84.75]</c:v>
+                  <c:v>[80.99-81.18]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[84.75-84.87]</c:v>
+                  <c:v>[81.18-81.38]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[84.87-84.99]</c:v>
+                  <c:v>[81.38-81.57]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2005,46 +2011,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>6</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
                 <c:pt idx="5">
-                  <c:v>9</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2181,46 +2187,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[83.64-83.76]</c:v>
+                  <c:v>[79.11-79.28]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[83.76-83.88]</c:v>
+                  <c:v>[79.28-79.46]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[83.88-84.0]</c:v>
+                  <c:v>[79.46-79.64]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[84.0-84.12]</c:v>
+                  <c:v>[79.64-79.82]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[84.12-84.24]</c:v>
+                  <c:v>[79.82-80.0]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[84.24-84.36]</c:v>
+                  <c:v>[80.0-80.17]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[84.36-84.48]</c:v>
+                  <c:v>[80.17-80.35]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[84.48-84.61]</c:v>
+                  <c:v>[80.35-80.53]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[84.61-84.73]</c:v>
+                  <c:v>[80.53-80.71]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[84.73-84.85]</c:v>
+                  <c:v>[80.71-80.89]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[84.85-84.97]</c:v>
+                  <c:v>[80.89-81.06]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[84.97-85.09]</c:v>
+                  <c:v>[81.06-81.24]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[85.09-85.21]</c:v>
+                  <c:v>[81.24-81.42]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[85.21-85.33]</c:v>
+                  <c:v>[81.42-81.6]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2232,46 +2238,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>20</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2409,31 +2415,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="4">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>31</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2448,28 +2454,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>55</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>22</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2597,31 +2603,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>23</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>24</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>27</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="7">
                   <c:v>28</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="8">
                   <c:v>30</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>34</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2639,22 +2645,22 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>1</c:v>
@@ -2785,31 +2791,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>25</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="3">
                   <c:v>26</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>28</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>29</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="6">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="7">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>33</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>34</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>36</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2824,28 +2830,28 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>43</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="6">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
                   <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>37</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2972,46 +2978,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.558-3.583]</c:v>
+                  <c:v>[3.471-3.504]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.583-3.608]</c:v>
+                  <c:v>[3.504-3.536]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.608-3.633]</c:v>
+                  <c:v>[3.536-3.568]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.633-3.657]</c:v>
+                  <c:v>[3.568-3.6]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.657-3.682]</c:v>
+                  <c:v>[3.6-3.632]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.682-3.707]</c:v>
+                  <c:v>[3.632-3.664]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.707-3.732]</c:v>
+                  <c:v>[3.664-3.697]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.732-3.757]</c:v>
+                  <c:v>[3.697-3.729]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.757-3.782]</c:v>
+                  <c:v>[3.729-3.761]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.782-3.806]</c:v>
+                  <c:v>[3.761-3.793]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.806-3.831]</c:v>
+                  <c:v>[3.793-3.825]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.831-3.856]</c:v>
+                  <c:v>[3.825-3.858]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[3.856-3.881]</c:v>
+                  <c:v>[3.858-3.89]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[3.881-3.906]</c:v>
+                  <c:v>[3.89-3.922]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3023,46 +3029,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>32</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>45</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>60</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>44</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>25</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3199,46 +3205,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.57-3.585]</c:v>
+                  <c:v>[3.471-3.493]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.585-3.6]</c:v>
+                  <c:v>[3.493-3.515]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.6-3.615]</c:v>
+                  <c:v>[3.515-3.537]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.615-3.63]</c:v>
+                  <c:v>[3.537-3.559]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.63-3.644]</c:v>
+                  <c:v>[3.559-3.582]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.644-3.659]</c:v>
+                  <c:v>[3.582-3.604]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.659-3.674]</c:v>
+                  <c:v>[3.604-3.626]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.674-3.689]</c:v>
+                  <c:v>[3.626-3.648]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.689-3.704]</c:v>
+                  <c:v>[3.648-3.67]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.704-3.718]</c:v>
+                  <c:v>[3.67-3.692]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.718-3.733]</c:v>
+                  <c:v>[3.692-3.714]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.733-3.748]</c:v>
+                  <c:v>[3.714-3.736]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[3.748-3.763]</c:v>
+                  <c:v>[3.736-3.758]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[3.763-3.778]</c:v>
+                  <c:v>[3.758-3.78]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3250,46 +3256,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>15</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3426,46 +3432,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.628-3.648]</c:v>
+                  <c:v>[3.555-3.581]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.648-3.667]</c:v>
+                  <c:v>[3.581-3.607]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.667-3.687]</c:v>
+                  <c:v>[3.607-3.633]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.687-3.707]</c:v>
+                  <c:v>[3.633-3.66]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.707-3.727]</c:v>
+                  <c:v>[3.66-3.686]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.727-3.747]</c:v>
+                  <c:v>[3.686-3.712]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.747-3.767]</c:v>
+                  <c:v>[3.712-3.738]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.767-3.787]</c:v>
+                  <c:v>[3.738-3.764]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.787-3.806]</c:v>
+                  <c:v>[3.764-3.791]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.806-3.826]</c:v>
+                  <c:v>[3.791-3.817]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.826-3.846]</c:v>
+                  <c:v>[3.817-3.843]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.846-3.866]</c:v>
+                  <c:v>[3.843-3.869]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[3.866-3.886]</c:v>
+                  <c:v>[3.869-3.896]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[3.886-3.906]</c:v>
+                  <c:v>[3.896-3.922]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3477,46 +3483,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3653,46 +3659,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[3.558-3.572]</c:v>
+                  <c:v>[3.481-3.502]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[3.572-3.585]</c:v>
+                  <c:v>[3.502-3.523]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[3.585-3.599]</c:v>
+                  <c:v>[3.523-3.544]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[3.599-3.613]</c:v>
+                  <c:v>[3.544-3.564]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[3.613-3.626]</c:v>
+                  <c:v>[3.564-3.585]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[3.626-3.64]</c:v>
+                  <c:v>[3.585-3.606]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[3.64-3.654]</c:v>
+                  <c:v>[3.606-3.627]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[3.654-3.667]</c:v>
+                  <c:v>[3.627-3.648]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[3.667-3.681]</c:v>
+                  <c:v>[3.648-3.669]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[3.681-3.694]</c:v>
+                  <c:v>[3.669-3.69]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[3.694-3.708]</c:v>
+                  <c:v>[3.69-3.71]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[3.708-3.722]</c:v>
+                  <c:v>[3.71-3.731]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[3.722-3.735]</c:v>
+                  <c:v>[3.731-3.752]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[3.735-3.749]</c:v>
+                  <c:v>[3.752-3.773]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3707,43 +3713,43 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="10">
                   <c:v>5</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>14</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>15</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>10</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6</c:v>
-                </c:pt>
                 <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3880,46 +3886,46 @@
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>[10.78-10.92]</c:v>
+                  <c:v>[11.08-11.23]</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>[10.92-11.07]</c:v>
+                  <c:v>[11.23-11.37]</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>[11.07-11.22]</c:v>
+                  <c:v>[11.37-11.52]</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>[11.22-11.37]</c:v>
+                  <c:v>[11.52-11.67]</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>[11.37-11.52]</c:v>
+                  <c:v>[11.67-11.82]</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>[11.52-11.67]</c:v>
+                  <c:v>[11.82-11.97]</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>[11.67-11.82]</c:v>
+                  <c:v>[11.97-12.11]</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>[11.82-11.97]</c:v>
+                  <c:v>[12.11-12.26]</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>[11.97-12.11]</c:v>
+                  <c:v>[12.26-12.41]</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>[12.11-12.26]</c:v>
+                  <c:v>[12.41-12.56]</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>[12.26-12.41]</c:v>
+                  <c:v>[12.56-12.71]</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>[12.41-12.56]</c:v>
+                  <c:v>[12.71-12.86]</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>[12.56-12.71]</c:v>
+                  <c:v>[12.86-13.0]</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>[12.71-12.86]</c:v>
+                  <c:v>[13.0-13.15]</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3931,46 +3937,46 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>32</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>41</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>57</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>44</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4920,79 +4926,79 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>18</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5">
-        <v>53</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B6">
-        <v>111</v>
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7">
-        <v>38</v>
+        <v>136</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>54</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B9">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -5022,7 +5028,7 @@
         <v>71</v>
       </c>
       <c r="B2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5030,7 +5036,7 @@
         <v>72</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5038,7 +5044,7 @@
         <v>73</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5046,7 +5052,7 @@
         <v>74</v>
       </c>
       <c r="B5">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5054,7 +5060,7 @@
         <v>75</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5062,7 +5068,7 @@
         <v>76</v>
       </c>
       <c r="B7">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5070,7 +5076,7 @@
         <v>77</v>
       </c>
       <c r="B8">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5078,7 +5084,7 @@
         <v>78</v>
       </c>
       <c r="B9">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5086,7 +5092,7 @@
         <v>79</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5094,7 +5100,7 @@
         <v>80</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5102,7 +5108,7 @@
         <v>81</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5118,7 +5124,7 @@
         <v>83</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5140,7 +5146,7 @@
         <v>84</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5148,7 +5154,7 @@
         <v>85</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5164,7 +5170,7 @@
         <v>87</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5172,7 +5178,7 @@
         <v>88</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5180,7 +5186,7 @@
         <v>89</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5188,7 +5194,7 @@
         <v>90</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5196,7 +5202,7 @@
         <v>91</v>
       </c>
       <c r="B8">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5204,7 +5210,7 @@
         <v>92</v>
       </c>
       <c r="B9">
-        <v>8</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5220,7 +5226,7 @@
         <v>94</v>
       </c>
       <c r="B11">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5228,7 +5234,7 @@
         <v>95</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5244,7 +5250,7 @@
         <v>97</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -5266,7 +5272,7 @@
         <v>98</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -5274,7 +5280,7 @@
         <v>99</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5290,7 +5296,7 @@
         <v>101</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5298,7 +5304,7 @@
         <v>102</v>
       </c>
       <c r="B5">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5306,7 +5312,7 @@
         <v>103</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5314,7 +5320,7 @@
         <v>104</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5322,7 +5328,7 @@
         <v>105</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5330,7 +5336,7 @@
         <v>106</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5338,7 +5344,7 @@
         <v>107</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5346,7 +5352,7 @@
         <v>108</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5354,20 +5360,20 @@
         <v>109</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>83</v>
+        <v>110</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B14">
         <v>2</v>
@@ -5389,114 +5395,114 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B1">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B5">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B6">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B7">
-        <v>28</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B8">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B9">
-        <v>54</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B10">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B11">
-        <v>30</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B12">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B13">
-        <v>6</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -5515,63 +5521,63 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -5579,7 +5585,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B9">
         <v>12</v>
@@ -5587,31 +5593,31 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B10">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B13">
         <v>2</v>
@@ -5619,7 +5625,7 @@
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -5641,63 +5647,63 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="B4">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B6">
-        <v>9</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B8">
         <v>11</v>
@@ -5705,50 +5711,50 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B9">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B10">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B11">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -5767,15 +5773,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B1">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -5783,98 +5789,98 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B8">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="B10">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B11">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -5893,7 +5899,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -5901,23 +5907,23 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>7</v>
@@ -5925,47 +5931,47 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B6">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B7">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -5984,7 +5990,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -5992,7 +5998,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -6000,55 +6006,55 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B3">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B6">
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8">
-        <v>9</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -6056,7 +6062,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -6075,7 +6081,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1">
         <v>0</v>
@@ -6083,71 +6089,71 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B8">
-        <v>37</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -6169,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6177,7 +6183,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6185,7 +6191,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>32</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6193,7 +6199,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>45</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6201,7 +6207,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>60</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6209,7 +6215,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6225,7 +6231,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6233,7 +6239,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6241,7 +6247,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6257,7 +6263,7 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6265,7 +6271,7 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6273,7 +6279,7 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -6295,7 +6301,7 @@
         <v>14</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6311,7 +6317,7 @@
         <v>16</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6319,7 +6325,7 @@
         <v>17</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6327,7 +6333,7 @@
         <v>18</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6335,7 +6341,7 @@
         <v>19</v>
       </c>
       <c r="B6">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6343,7 +6349,7 @@
         <v>20</v>
       </c>
       <c r="B7">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6351,7 +6357,7 @@
         <v>21</v>
       </c>
       <c r="B8">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6359,7 +6365,7 @@
         <v>22</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6367,7 +6373,7 @@
         <v>23</v>
       </c>
       <c r="B10">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6375,7 +6381,7 @@
         <v>24</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6383,7 +6389,7 @@
         <v>25</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6399,7 +6405,7 @@
         <v>27</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6421,7 +6427,7 @@
         <v>28</v>
       </c>
       <c r="B1">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6437,7 +6443,7 @@
         <v>30</v>
       </c>
       <c r="B3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6445,7 +6451,7 @@
         <v>31</v>
       </c>
       <c r="B4">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6453,7 +6459,7 @@
         <v>32</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6461,7 +6467,7 @@
         <v>33</v>
       </c>
       <c r="B6">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6469,7 +6475,7 @@
         <v>34</v>
       </c>
       <c r="B7">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6485,7 +6491,7 @@
         <v>36</v>
       </c>
       <c r="B9">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6493,7 +6499,7 @@
         <v>37</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6501,7 +6507,7 @@
         <v>38</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6509,7 +6515,7 @@
         <v>39</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6517,7 +6523,7 @@
         <v>40</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6525,7 +6531,7 @@
         <v>41</v>
       </c>
       <c r="B14">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6555,7 +6561,7 @@
         <v>43</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -6563,7 +6569,7 @@
         <v>44</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6571,7 +6577,7 @@
         <v>45</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6579,7 +6585,7 @@
         <v>46</v>
       </c>
       <c r="B5">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6587,7 +6593,7 @@
         <v>47</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6595,7 +6601,7 @@
         <v>48</v>
       </c>
       <c r="B7">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6603,7 +6609,7 @@
         <v>49</v>
       </c>
       <c r="B8">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6611,7 +6617,7 @@
         <v>50</v>
       </c>
       <c r="B9">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6619,7 +6625,7 @@
         <v>51</v>
       </c>
       <c r="B10">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6627,7 +6633,7 @@
         <v>52</v>
       </c>
       <c r="B11">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6635,7 +6641,7 @@
         <v>53</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6643,7 +6649,7 @@
         <v>54</v>
       </c>
       <c r="B13">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6651,7 +6657,7 @@
         <v>55</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -6673,7 +6679,7 @@
         <v>56</v>
       </c>
       <c r="B1">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6689,7 +6695,7 @@
         <v>58</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -6697,7 +6703,7 @@
         <v>59</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -6705,7 +6711,7 @@
         <v>60</v>
       </c>
       <c r="B5">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -6713,7 +6719,7 @@
         <v>61</v>
       </c>
       <c r="B6">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -6721,7 +6727,7 @@
         <v>62</v>
       </c>
       <c r="B7">
-        <v>24</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -6729,7 +6735,7 @@
         <v>63</v>
       </c>
       <c r="B8">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -6737,7 +6743,7 @@
         <v>64</v>
       </c>
       <c r="B9">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -6745,7 +6751,7 @@
         <v>65</v>
       </c>
       <c r="B10">
-        <v>57</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -6753,7 +6759,7 @@
         <v>66</v>
       </c>
       <c r="B11">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6761,7 +6767,7 @@
         <v>67</v>
       </c>
       <c r="B12">
-        <v>34</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -6769,7 +6775,7 @@
         <v>68</v>
       </c>
       <c r="B13">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -6777,7 +6783,7 @@
         <v>69</v>
       </c>
       <c r="B14">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>